<commit_message>
major updates matching the Frontiers submission
</commit_message>
<xml_diff>
--- a/VennOutput/NonTrimmed_MODERNA_Combined_Output_Mono-vs-Bivalent.xlsx
+++ b/VennOutput/NonTrimmed_MODERNA_Combined_Output_Mono-vs-Bivalent.xlsx
@@ -370,52 +370,52 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Case No.x</t>
+          <t>Case No</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>PRR.x</t>
+          <t>PRR</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Percentage of cases.x</t>
+          <t>Percentage of cases</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Xsquared.x</t>
+          <t>Xsquared</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Significance.x</t>
+          <t>Significance</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Case No.y</t>
+          <t>Case No.MODERNA_BI</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>PRR.y</t>
+          <t>PRR.MODERNA_BI</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Percentage of cases.y</t>
+          <t>Percentage of cases.MODERNA_BI</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Xsquared.y</t>
+          <t>Xsquared.MODERNA_BI</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Significance.y</t>
+          <t>Significance.MODERNA_BI</t>
         </is>
       </c>
     </row>

</xml_diff>